<commit_message>
change speed to reach valid solution
- process time / 2
- every agent go to TOP
</commit_message>
<xml_diff>
--- a/data/therblig_process_time.xlsx
+++ b/data/therblig_process_time.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Document\NTHU\master\HRC_taskalloc_w.TB_w.AR\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuyulu\Documents\thesis\HRC_taskAlloc_w.TB_w.AR\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD432815-6FCD-4A88-8760-A8B540C9BFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F44A6E-A883-4113-AE76-114DA77C2E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18150" yWindow="10200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -535,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -544,6 +553,7 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -571,7 +581,7 @@
         <v>20</v>
       </c>
       <c r="D2" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -585,7 +595,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="1">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -599,7 +609,7 @@
         <v>45</v>
       </c>
       <c r="D4" s="1">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -613,7 +623,7 @@
         <v>55</v>
       </c>
       <c r="D5" s="1">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +637,7 @@
         <v>61</v>
       </c>
       <c r="D6" s="1">
-        <v>111</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +651,7 @@
         <v>64</v>
       </c>
       <c r="D7" s="1">
-        <v>133</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,7 +665,7 @@
         <v>68</v>
       </c>
       <c r="D8" s="1">
-        <v>156</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -669,7 +679,7 @@
         <v>71</v>
       </c>
       <c r="D9" s="1">
-        <v>178</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -683,7 +693,7 @@
         <v>75</v>
       </c>
       <c r="D10" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -697,7 +707,7 @@
         <v>78</v>
       </c>
       <c r="D11" s="1">
-        <v>222</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -711,7 +721,7 @@
         <v>81</v>
       </c>
       <c r="D12" s="1">
-        <v>244</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -725,7 +735,7 @@
         <v>85</v>
       </c>
       <c r="D13" s="1">
-        <v>267</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -739,7 +749,7 @@
         <v>88</v>
       </c>
       <c r="D14" s="1">
-        <v>289</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -753,7 +763,7 @@
         <v>92</v>
       </c>
       <c r="D15" s="1">
-        <v>311</v>
+        <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -767,7 +777,7 @@
         <v>95</v>
       </c>
       <c r="D16" s="1">
-        <v>333</v>
+        <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -781,7 +791,7 @@
         <v>20</v>
       </c>
       <c r="D17" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -795,7 +805,7 @@
         <v>34</v>
       </c>
       <c r="D18" s="1">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,7 +819,7 @@
         <v>45</v>
       </c>
       <c r="D19" s="1">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,7 +833,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="1">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,7 +847,7 @@
         <v>63</v>
       </c>
       <c r="D21" s="1">
-        <v>111</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,7 +861,7 @@
         <v>74</v>
       </c>
       <c r="D22" s="1">
-        <v>133</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -865,7 +875,7 @@
         <v>82</v>
       </c>
       <c r="D23" s="1">
-        <v>156</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -879,7 +889,7 @@
         <v>88</v>
       </c>
       <c r="D24" s="1">
-        <v>178</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -893,7 +903,7 @@
         <v>94</v>
       </c>
       <c r="D25" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -907,7 +917,7 @@
         <v>100</v>
       </c>
       <c r="D26" s="1">
-        <v>222</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,7 +931,7 @@
         <v>105</v>
       </c>
       <c r="D27" s="1">
-        <v>244</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,7 +945,7 @@
         <v>111</v>
       </c>
       <c r="D28" s="1">
-        <v>267</v>
+        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -949,7 +959,7 @@
         <v>117</v>
       </c>
       <c r="D29" s="1">
-        <v>289</v>
+        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -963,7 +973,7 @@
         <v>122</v>
       </c>
       <c r="D30" s="1">
-        <v>311</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -977,7 +987,7 @@
         <v>128</v>
       </c>
       <c r="D31" s="1">
-        <v>333</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -991,7 +1001,7 @@
         <v>20</v>
       </c>
       <c r="D32" s="1">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1005,7 +1015,7 @@
         <v>40</v>
       </c>
       <c r="D33" s="1">
-        <v>44</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1019,7 +1029,7 @@
         <v>50</v>
       </c>
       <c r="D34" s="1">
-        <v>67</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1033,7 +1043,7 @@
         <v>58.999999999999993</v>
       </c>
       <c r="D35" s="1">
-        <v>89</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1047,7 +1057,7 @@
         <v>68</v>
       </c>
       <c r="D36" s="1">
-        <v>111</v>
+        <v>56</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1061,7 +1071,7 @@
         <v>77</v>
       </c>
       <c r="D37" s="1">
-        <v>133</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1085,7 @@
         <v>85</v>
       </c>
       <c r="D38" s="1">
-        <v>156</v>
+        <v>78</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1089,7 +1099,7 @@
         <v>92</v>
       </c>
       <c r="D39" s="1">
-        <v>178</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,7 +1113,7 @@
         <v>98</v>
       </c>
       <c r="D40" s="1">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1117,7 +1127,7 @@
         <v>105</v>
       </c>
       <c r="D41" s="1">
-        <v>222</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1131,7 +1141,7 @@
         <v>112.00000000000001</v>
       </c>
       <c r="D42" s="1">
-        <v>244</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1145,7 +1155,7 @@
         <v>117.99999999999999</v>
       </c>
       <c r="D43" s="1">
-        <v>267</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1159,7 +1169,7 @@
         <v>123.00000000000001</v>
       </c>
       <c r="D44" s="1">
-        <v>289</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1173,7 +1183,7 @@
         <v>128</v>
       </c>
       <c r="D45" s="1">
-        <v>311</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1187,7 +1197,7 @@
         <v>133</v>
       </c>
       <c r="D46" s="1">
-        <v>333</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>